<commit_message>
added file figures/Table 1 - Stratified by Health Status and Sex/Table 1 - Stratified by Health Status and Sex.xlsx
</commit_message>
<xml_diff>
--- a/figures/Table 1 - Stratified by Health Status and Sex/Table 1 - Stratified by Health Status and Sex.xlsx
+++ b/figures/Table 1 - Stratified by Health Status and Sex/Table 1 - Stratified by Health Status and Sex.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
-  <si>
-    <t>Table 1 - Stratified by Health Status and Sex</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t xml:space="preserve">           </t>
   </si>
@@ -28,31 +25,31 @@
     <t>p value</t>
   </si>
   <si>
+    <t xml:space="preserve">n        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Group (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- COPD  </t>
+  </si>
+  <si>
+    <t>8 (44.4)</t>
+  </si>
+  <si>
+    <t>10 (31.2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">n        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t>Group (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- COPD  </t>
-  </si>
-  <si>
-    <t>8 (44.4)</t>
-  </si>
-  <si>
-    <t>10 (31.2)</t>
   </si>
   <si>
     <t>- HEALTHY</t>
@@ -107,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -115,6 +112,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -131,7 +133,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,34 +146,13 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -185,7 +166,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -194,73 +175,13 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -270,47 +191,26 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -330,10 +230,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -350,10 +249,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -530,11 +429,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -543,27 +445,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -820,10 +722,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1114,7 +1016,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1395,226 +1297,146 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G12"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.35156" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.35156" style="1" customWidth="1"/>
-    <col min="8" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85156" style="1" customWidth="1"/>
+    <col min="5" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.05" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" ht="17.55" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.028</v>
+      </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s" s="9">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="G4" s="11"/>
+      <c r="A4" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="12">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13">
-        <v>18</v>
-      </c>
-      <c r="D5" s="13">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s" s="10">
-        <v>8</v>
+      <c r="A5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.028</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" t="s" s="10">
-        <v>8</v>
+      <c r="A6" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" t="s" s="10">
-        <v>8</v>
+      <c r="A7" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.019</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" t="s" s="10">
-        <v>8</v>
+      <c r="A8" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.216</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" t="s" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.019</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" t="s" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s" s="10">
+      <c r="A9" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="E11" s="13">
-        <v>0.216</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" t="s" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" t="s" s="8">
+      <c r="B9" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="C12" t="s" s="10">
+      <c r="C9" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="D12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="D9" s="5">
         <v>0.638</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>